<commit_message>
Final resutlts with tables with the analysis included
</commit_message>
<xml_diff>
--- a/Results/Final Results/Samples/600Scen/Results_Sample600_01.xlsx
+++ b/Results/Final Results/Samples/600Scen/Results_Sample600_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\6.Semester\Bachelor-Arbeit\bachelor-thesis\bachelor-thesis\Results\Final Results\Samples\600Scen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2F712B-1755-470A-98FA-BD700F1C7E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A395B100-CE3F-4F84-8ED7-B268BE71BFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <dimension ref="A1:S121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,10 +1018,11 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1.107E-2</v>
+        <f>(TestingFile3[[#This Row],[Obj. LR]]-TestingFile3[[#This Row],[LB Heuristic]])/TestingFile3[[#This Row],[Obj. LR]]</f>
+        <v>1.2177177027362731E-2</v>
       </c>
       <c r="H7">
         <v>7.1000000000000002E-4</v>
@@ -1030,19 +1031,20 @@
         <v>251.56241</v>
       </c>
       <c r="J7">
-        <v>251.27977000000001</v>
+        <v>251.56241</v>
       </c>
       <c r="K7">
-        <v>-1.1199999999999999E-3</v>
+        <f>(TestingFile3[[#This Row],[Obj. LR]]-TestingFile3[[#This Row],[Obj. Naive]])/TestingFile3[[#This Row],[Obj. LR]]</f>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>1270</v>
       </c>
       <c r="M7">
-        <v>3626</v>
+        <v>248</v>
       </c>
       <c r="N7">
-        <v>1.9533799999999999</v>
+        <v>0.84111000000000002</v>
       </c>
       <c r="O7">
         <v>248.49909</v>

</xml_diff>